<commit_message>
Cambio en la plantilla, final
</commit_message>
<xml_diff>
--- a/docs/Plantilla.xlsx
+++ b/docs/Plantilla.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\communityRiskAnalytics\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F972F9-4ECE-4102-BE6C-427BC0600824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5E4E7A-7CB9-4FCE-9598-0BFD6C1F93EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="G/G9V8ynvvk9Giwx9DuS95ohqICxHQ+cziO6Tk8YV3d60xsU1dbc0S0kzRKfpXP3i5+Bi/kRbOE1rocjhqAm3A==" workbookSaltValue="Y69OzHk9rastx3U/PXWspg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -73,31 +73,30 @@
     <t>Resultado antes de impuestos</t>
   </si>
   <si>
+    <t>Deudores comerciales y cuentas a cobrar</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Estados financieros 2022
+      <t xml:space="preserve">Estados financieros CRA
 </t>
     </r>
     <r>
       <rPr>
         <u/>
-        <sz val="8"/>
+        <sz val="9"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
-      <t>Rellene solo los campos en gris</t>
+      <t>Rellene solo los campos de color azul</t>
     </r>
-  </si>
-  <si>
-    <t>Deudores comerciales y cuentas a cobrar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,27 +105,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -138,7 +140,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.499984740745262"/>
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -265,23 +267,23 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="4" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,117 +567,117 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="11" max="11" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="9"/>
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2"/>
       <c r="K1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="7"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="6"/>
+      <c r="A3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="8"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="8"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="8"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="8"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6"/>
+      <c r="B7" s="8"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="8"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="6"/>
+      <c r="B9" s="8"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="8"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="8"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="8"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="6"/>
+      <c r="B13" s="8"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="8"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="6"/>
+      <c r="B15" s="8"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="7"/>
+      <c r="B16" s="9"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="QqOfwuFKNOeTJjdarq3sfy7N3S221zjVvvm9CgS3PKzc86HvkBFLQM4iH8SB8qcqLPBhUhNWsVIXekV0vs+shQ==" saltValue="oz4i/Via2OyNnWJU8yRi/w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="IPuT1BB0HHO7h/WLcNE8bno9rp5G/AlRBCaCJSp/DS/eqPnukV0DZ2DnY4rIBH8laljmQmrRnniNar5RYoDVEw==" saltValue="10HTp7drJ3Dx7DRs6BVWdA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
     <protectedRange sqref="B2:B16" name="Editables"/>
   </protectedRanges>

</xml_diff>